<commit_message>
Fixed bugs and added comment in Arduino
</commit_message>
<xml_diff>
--- a/Figures/Communication protocol.xlsx
+++ b/Figures/Communication protocol.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\valen\Google Drive\INSA 2A\S4\P2I\Ressources projet\schem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C7E70E7-7996-4132-9373-91A122E86D12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6524165-4454-4B8E-ABFF-3E7AFC04BF2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9DEAF87A-190C-4914-965F-722D1C4CC653}"/>
   </bookViews>
@@ -166,9 +166,6 @@
     <t>This helps to interpret the message more easily in arduino</t>
   </si>
   <si>
-    <t>Purpose</t>
-  </si>
-  <si>
     <t>Stop a pause</t>
   </si>
   <si>
@@ -230,6 +227,9 @@
   </si>
   <si>
     <t>Sent by the app</t>
+  </si>
+  <si>
+    <t>Instruction</t>
   </si>
 </sst>
 </file>
@@ -523,7 +523,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -594,6 +594,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -778,7 +782,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{582EB0E4-3935-49C2-A14F-0D4C22C3C9DC}" name="Tableau1" displayName="Tableau1" ref="B6:F34" headerRowCount="0" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10" tableBorderDxfId="9" totalsRowBorderDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{582EB0E4-3935-49C2-A14F-0D4C22C3C9DC}" name="Tableau1" displayName="Tableau1" ref="B6:F24" headerRowCount="0" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10" tableBorderDxfId="9" totalsRowBorderDxfId="8">
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{D9CD111F-CF26-4D0D-95E3-2D4B9CA4E2C0}" name="Colonne1" dataDxfId="7"/>
     <tableColumn id="2" xr3:uid="{82C9F2FD-43A6-47CC-B123-5953133616DD}" name="Colonne2" dataDxfId="6"/>
@@ -1087,10 +1091,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89FF181A-B047-4DD6-A7C0-148D426E8686}">
-  <dimension ref="B1:H34"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="B6" sqref="B6:F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1110,7 +1114,7 @@
       </c>
       <c r="C2" s="27"/>
       <c r="D2" s="25" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E2" s="26"/>
       <c r="F2" s="26"/>
@@ -1123,7 +1127,7 @@
       </c>
       <c r="C3" s="32"/>
       <c r="D3" s="28" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E3" s="29"/>
       <c r="F3" s="29"/>
@@ -1136,7 +1140,7 @@
       </c>
       <c r="C4" s="33"/>
       <c r="D4" s="30" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E4" s="31"/>
       <c r="F4" s="31"/>
@@ -1146,7 +1150,7 @@
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
       <c r="C6" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2" t="s">
@@ -1156,7 +1160,7 @@
     </row>
     <row r="7" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="16" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="C7" s="17" t="s">
         <v>38</v>
@@ -1324,7 +1328,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B17" s="4" t="s">
         <v>34</v>
       </c>
@@ -1341,7 +1345,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B18" s="4" t="s">
         <v>35</v>
       </c>
@@ -1358,7 +1362,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B19" s="4" t="s">
         <v>36</v>
       </c>
@@ -1375,7 +1379,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B20" s="4" t="s">
         <v>37</v>
       </c>
@@ -1392,9 +1396,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B21" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C21" s="9" t="s">
         <v>24</v>
@@ -1409,126 +1413,166 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B22" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D22" s="6" t="s">
         <v>8</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F22" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B23" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E23" s="6" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B23" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="E23" s="6" t="s">
-        <v>47</v>
-      </c>
       <c r="F23" s="7" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B24" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B24" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C24" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="C24" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="D24" s="6" t="s">
+      <c r="D24" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="E24" s="6" t="s">
+      <c r="E24" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="F24" s="7" t="s">
+      <c r="F24" s="11" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B25" s="4"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="7"/>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B26" s="4"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="7"/>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B27" s="4"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="7"/>
-    </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B28" s="4"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="7"/>
-    </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B29" s="4"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="7"/>
-    </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B30" s="4"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="7"/>
-    </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B31" s="4"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
-      <c r="F31" s="7"/>
-    </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B32" s="4"/>
-      <c r="C32" s="5"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="6"/>
-      <c r="F32" s="7"/>
-    </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B33" s="4"/>
-      <c r="C33" s="5"/>
-      <c r="D33" s="6"/>
-      <c r="E33" s="6"/>
-      <c r="F33" s="7"/>
-    </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B34" s="8"/>
-      <c r="C34" s="9"/>
-      <c r="D34" s="10"/>
-      <c r="E34" s="10"/>
-      <c r="F34" s="11"/>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="34"/>
+      <c r="B25" s="34"/>
+      <c r="C25" s="34"/>
+      <c r="D25" s="35"/>
+      <c r="E25" s="35"/>
+      <c r="F25" s="35"/>
+      <c r="G25" s="34"/>
+      <c r="H25" s="34"/>
+      <c r="I25" s="34"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="34"/>
+      <c r="B26" s="34"/>
+      <c r="C26" s="34"/>
+      <c r="D26" s="35"/>
+      <c r="E26" s="35"/>
+      <c r="F26" s="35"/>
+      <c r="G26" s="34"/>
+      <c r="H26" s="34"/>
+      <c r="I26" s="34"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="34"/>
+      <c r="B27" s="34"/>
+      <c r="C27" s="34"/>
+      <c r="D27" s="35"/>
+      <c r="E27" s="35"/>
+      <c r="F27" s="35"/>
+      <c r="G27" s="34"/>
+      <c r="H27" s="34"/>
+      <c r="I27" s="34"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="34"/>
+      <c r="B28" s="34"/>
+      <c r="C28" s="34"/>
+      <c r="D28" s="35"/>
+      <c r="E28" s="35"/>
+      <c r="F28" s="35"/>
+      <c r="G28" s="34"/>
+      <c r="H28" s="34"/>
+      <c r="I28" s="34"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="34"/>
+      <c r="B29" s="34"/>
+      <c r="C29" s="34"/>
+      <c r="D29" s="35"/>
+      <c r="E29" s="35"/>
+      <c r="F29" s="35"/>
+      <c r="G29" s="34"/>
+      <c r="H29" s="34"/>
+      <c r="I29" s="34"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="34"/>
+      <c r="B30" s="34"/>
+      <c r="C30" s="34"/>
+      <c r="D30" s="35"/>
+      <c r="E30" s="35"/>
+      <c r="F30" s="35"/>
+      <c r="G30" s="34"/>
+      <c r="H30" s="34"/>
+      <c r="I30" s="34"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="34"/>
+      <c r="B31" s="34"/>
+      <c r="C31" s="34"/>
+      <c r="D31" s="35"/>
+      <c r="E31" s="35"/>
+      <c r="F31" s="35"/>
+      <c r="G31" s="34"/>
+      <c r="H31" s="34"/>
+      <c r="I31" s="34"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="34"/>
+      <c r="B32" s="34"/>
+      <c r="C32" s="34"/>
+      <c r="D32" s="35"/>
+      <c r="E32" s="35"/>
+      <c r="F32" s="35"/>
+      <c r="G32" s="34"/>
+      <c r="H32" s="34"/>
+      <c r="I32" s="34"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="34"/>
+      <c r="B33" s="34"/>
+      <c r="C33" s="34"/>
+      <c r="D33" s="35"/>
+      <c r="E33" s="35"/>
+      <c r="F33" s="35"/>
+      <c r="G33" s="34"/>
+      <c r="H33" s="34"/>
+      <c r="I33" s="34"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="34"/>
+      <c r="B34" s="34"/>
+      <c r="C34" s="34"/>
+      <c r="D34" s="35"/>
+      <c r="E34" s="35"/>
+      <c r="F34" s="35"/>
+      <c r="G34" s="34"/>
+      <c r="H34" s="34"/>
+      <c r="I34" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>